<commit_message>
small update of analysis
</commit_message>
<xml_diff>
--- a/data/2019_25_11 Thésaurus version pour osiris 2019 PL - English Traduction.xlsx
+++ b/data/2019_25_11 Thésaurus version pour osiris 2019 PL - English Traduction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\Downloads\Extraction_InformationsPatients-20200702T221646Z-001\Extraction_InformationsPatients\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\exalis\github\projet_aura_classification\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83284B8-C202-474F-A9B9-39BDD56E14E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A3B891-F4DE-4AF4-9BC3-97244AA0A086}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="720">
   <si>
     <t>DCD</t>
   </si>
@@ -2234,6 +2234,12 @@
   </si>
   <si>
     <t>English traduction</t>
+  </si>
+  <si>
+    <t>Généralisée</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -2493,10 +2499,16 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -2507,12 +2519,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3175,17 +3181,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C53:D53"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C53:D53"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
@@ -3197,10 +3203,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BA85"/>
+  <dimension ref="A1:BA85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3220,52 +3226,52 @@
         <v>264</v>
       </c>
       <c r="D1" s="27"/>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="46" t="s">
         <v>251</v>
       </c>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="50"/>
-      <c r="AE1" s="50"/>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="50"/>
-      <c r="AH1" s="50"/>
-      <c r="AI1" s="50"/>
-      <c r="AJ1" s="50"/>
-      <c r="AK1" s="50"/>
-      <c r="AL1" s="50"/>
-      <c r="AM1" s="50"/>
-      <c r="AN1" s="50"/>
-      <c r="AO1" s="50"/>
-      <c r="AP1" s="50"/>
-      <c r="AQ1" s="50"/>
-      <c r="AR1" s="50"/>
-      <c r="AS1" s="50"/>
-      <c r="AT1" s="50"/>
-      <c r="AU1" s="50"/>
-      <c r="AV1" s="50"/>
-      <c r="AW1" s="50"/>
-      <c r="AX1" s="50"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
+      <c r="AW1" s="46"/>
+      <c r="AX1" s="46"/>
     </row>
     <row r="2" spans="2:53" x14ac:dyDescent="0.35">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="47"/>
+      <c r="C2" s="49"/>
       <c r="D2" s="43" t="s">
         <v>717</v>
       </c>
@@ -3299,14 +3305,14 @@
       <c r="S2" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="T2" s="46" t="s">
+      <c r="T2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
       <c r="Z2" t="s">
         <v>484</v>
       </c>
@@ -3353,12 +3359,12 @@
       <c r="AT2" s="29" t="s">
         <v>482</v>
       </c>
-      <c r="AU2" s="46" t="s">
+      <c r="AU2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="AV2" s="46"/>
-      <c r="AW2" s="46"/>
-      <c r="AX2" s="46"/>
+      <c r="AV2" s="45"/>
+      <c r="AW2" s="45"/>
+      <c r="AX2" s="45"/>
       <c r="AY2" s="39" t="s">
         <v>484</v>
       </c>
@@ -3411,22 +3417,22 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
-      <c r="T4" s="45" t="s">
+      <c r="T4" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
       <c r="Y4" s="14"/>
-      <c r="AD4" s="45" t="s">
+      <c r="AD4" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="AE4" s="45"/>
-      <c r="AF4" s="45"/>
-      <c r="AG4" s="45"/>
-      <c r="AH4" s="45"/>
-      <c r="AI4" s="45"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
+      <c r="AG4" s="48"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="48"/>
       <c r="AN4" s="2" t="s">
         <v>451</v>
       </c>
@@ -3578,12 +3584,12 @@
       <c r="AT6" s="29">
         <v>999</v>
       </c>
-      <c r="AU6" s="46" t="s">
+      <c r="AU6" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="AV6" s="46"/>
-      <c r="AW6" s="46"/>
-      <c r="AX6" s="46"/>
+      <c r="AV6" s="45"/>
+      <c r="AW6" s="45"/>
+      <c r="AX6" s="45"/>
       <c r="AY6" s="39" t="s">
         <v>484</v>
       </c>
@@ -3600,11 +3606,11 @@
         <v>19</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="I7" s="51" t="s">
+      <c r="I7" s="47" t="s">
         <v>250</v>
       </c>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
       <c r="M7" s="2" t="s">
         <v>328</v>
       </c>
@@ -3680,11 +3686,11 @@
       <c r="G8" s="37">
         <v>36387</v>
       </c>
-      <c r="I8" s="49" t="s">
+      <c r="I8" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
       <c r="M8" s="2" t="s">
         <v>329</v>
       </c>
@@ -4305,13 +4311,13 @@
       </c>
       <c r="Q16" s="36"/>
       <c r="R16" s="11"/>
-      <c r="T16" s="45" t="s">
+      <c r="T16" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="45"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
       <c r="Y16" s="14"/>
       <c r="AA16" s="39"/>
       <c r="AD16" s="28" t="s">
@@ -4333,7 +4339,7 @@
       <c r="AQ16" s="39"/>
       <c r="AR16" s="39"/>
     </row>
-    <row r="17" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B17" s="2"/>
       <c r="C17" s="5" t="s">
         <v>24</v>
@@ -4383,7 +4389,7 @@
       <c r="AQ17" s="39"/>
       <c r="AR17" s="39"/>
     </row>
-    <row r="18" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>274</v>
       </c>
@@ -4447,7 +4453,7 @@
       <c r="AQ18" s="39"/>
       <c r="AR18" s="39"/>
     </row>
-    <row r="19" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:44" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>275</v>
       </c>
@@ -4514,7 +4520,7 @@
       <c r="AQ19" s="39"/>
       <c r="AR19" s="39"/>
     </row>
-    <row r="20" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B20" s="28" t="s">
         <v>276</v>
       </c>
@@ -4589,7 +4595,10 @@
       </c>
       <c r="AR20" s="39"/>
     </row>
-    <row r="21" spans="2:44" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:44" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>718</v>
+      </c>
       <c r="B21" s="28" t="s">
         <v>277</v>
       </c>
@@ -4660,7 +4669,7 @@
       </c>
       <c r="AR21" s="39"/>
     </row>
-    <row r="22" spans="2:44" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:44" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="28" t="s">
         <v>278</v>
       </c>
@@ -4722,7 +4731,10 @@
       </c>
       <c r="AR22" s="39"/>
     </row>
-    <row r="23" spans="2:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>718</v>
+      </c>
       <c r="B23" s="28" t="s">
         <v>279</v>
       </c>
@@ -4788,7 +4800,10 @@
       <c r="AQ23" s="39"/>
       <c r="AR23" s="39"/>
     </row>
-    <row r="24" spans="2:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>718</v>
+      </c>
       <c r="B24" s="28" t="s">
         <v>280</v>
       </c>
@@ -4864,7 +4879,10 @@
       </c>
       <c r="AR24" s="39"/>
     </row>
-    <row r="25" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>718</v>
+      </c>
       <c r="B25" s="28" t="s">
         <v>281</v>
       </c>
@@ -4938,7 +4956,10 @@
       </c>
       <c r="AR25" s="39"/>
     </row>
-    <row r="26" spans="2:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>718</v>
+      </c>
       <c r="B26" s="28" t="s">
         <v>282</v>
       </c>
@@ -5006,7 +5027,7 @@
       </c>
       <c r="AR26" s="39"/>
     </row>
-    <row r="27" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="28" t="s">
         <v>283</v>
       </c>
@@ -5081,7 +5102,7 @@
       </c>
       <c r="AR27" s="39"/>
     </row>
-    <row r="28" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B28" s="28" t="s">
         <v>284</v>
       </c>
@@ -5157,7 +5178,10 @@
       </c>
       <c r="AR28" s="39"/>
     </row>
-    <row r="29" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>718</v>
+      </c>
       <c r="B29" s="28" t="s">
         <v>285</v>
       </c>
@@ -5233,7 +5257,7 @@
       </c>
       <c r="AR29" s="39"/>
     </row>
-    <row r="30" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B30" s="28" t="s">
         <v>286</v>
       </c>
@@ -5309,7 +5333,7 @@
       </c>
       <c r="AR30" s="39"/>
     </row>
-    <row r="31" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
       <c r="C31" s="5" t="s">
         <v>56</v>
@@ -5372,7 +5396,10 @@
       </c>
       <c r="AR31" s="39"/>
     </row>
-    <row r="32" spans="2:44" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>718</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>287</v>
       </c>
@@ -5431,7 +5458,10 @@
       </c>
       <c r="AR32" s="39"/>
     </row>
-    <row r="33" spans="2:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:37" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>718</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>288</v>
       </c>
@@ -5478,13 +5508,13 @@
       <c r="AD33" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="AE33" s="48" t="s">
+      <c r="AE33" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="AF33" s="48"/>
-      <c r="AG33" s="48"/>
-      <c r="AH33" s="48"/>
-      <c r="AI33" s="48"/>
+      <c r="AF33" s="50"/>
+      <c r="AG33" s="50"/>
+      <c r="AH33" s="50"/>
+      <c r="AI33" s="50"/>
       <c r="AJ33" s="39" t="s">
         <v>586</v>
       </c>
@@ -5492,7 +5522,10 @@
         <v>549</v>
       </c>
     </row>
-    <row r="34" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>718</v>
+      </c>
       <c r="B34" s="28" t="s">
         <v>289</v>
       </c>
@@ -5529,7 +5562,7 @@
         <v>98892</v>
       </c>
     </row>
-    <row r="35" spans="2:37" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:37" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="28" t="s">
         <v>290</v>
       </c>
@@ -5577,7 +5610,10 @@
         <v>99796</v>
       </c>
     </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>718</v>
+      </c>
       <c r="B36" s="28" t="s">
         <v>291</v>
       </c>
@@ -5609,7 +5645,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B37" s="28" t="s">
         <v>292</v>
       </c>
@@ -5642,7 +5678,10 @@
         <v>48471</v>
       </c>
     </row>
-    <row r="38" spans="2:37" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:37" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>718</v>
+      </c>
       <c r="B38" s="28" t="s">
         <v>518</v>
       </c>
@@ -5679,7 +5718,7 @@
         <v>48471</v>
       </c>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B39" s="2"/>
       <c r="C39" s="5" t="s">
         <v>30</v>
@@ -5705,7 +5744,7 @@
         <v>48471</v>
       </c>
     </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:37" ht="29" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>293</v>
       </c>
@@ -5737,7 +5776,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="41" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>294</v>
       </c>
@@ -5770,7 +5809,7 @@
         <v>268940</v>
       </c>
     </row>
-    <row r="42" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:37" ht="29" x14ac:dyDescent="0.35">
       <c r="B42" s="28" t="s">
         <v>295</v>
       </c>
@@ -5800,7 +5839,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B43" s="28" t="s">
         <v>296</v>
       </c>
@@ -5833,7 +5872,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="44" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B44" s="28" t="s">
         <v>297</v>
       </c>
@@ -5862,7 +5901,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="45" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B45" s="28" t="s">
         <v>298</v>
       </c>
@@ -5895,7 +5934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B46" s="28" t="s">
         <v>299</v>
       </c>
@@ -5928,7 +5967,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="47" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B47" s="28" t="s">
         <v>300</v>
       </c>
@@ -5963,7 +6002,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B48" s="28" t="s">
         <v>301</v>
       </c>
@@ -5998,7 +6037,7 @@
         <v>2836</v>
       </c>
     </row>
-    <row r="49" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B49" s="2"/>
       <c r="C49" s="5" t="s">
         <v>66</v>
@@ -6020,7 +6059,7 @@
         <v>98889</v>
       </c>
     </row>
-    <row r="50" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
         <v>302</v>
       </c>
@@ -6049,7 +6088,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="51" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B51" s="9" t="s">
         <v>303</v>
       </c>
@@ -6066,17 +6105,17 @@
         <v>536</v>
       </c>
       <c r="S51" s="16"/>
-      <c r="T51" s="45" t="s">
+      <c r="T51" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="U51" s="45"/>
-      <c r="V51" s="45"/>
-      <c r="W51" s="45"/>
-      <c r="X51" s="45"/>
+      <c r="U51" s="48"/>
+      <c r="V51" s="48"/>
+      <c r="W51" s="48"/>
+      <c r="X51" s="48"/>
       <c r="Y51" s="14"/>
       <c r="AA51" s="39"/>
     </row>
-    <row r="52" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B52" s="28" t="s">
         <v>304</v>
       </c>
@@ -6106,7 +6145,7 @@
       </c>
       <c r="AC52" s="23"/>
     </row>
-    <row r="53" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B53" s="21" t="s">
         <v>305</v>
       </c>
@@ -6135,7 +6174,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B54" s="28" t="s">
         <v>306</v>
       </c>
@@ -6164,7 +6203,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="55" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B55" s="21" t="s">
         <v>307</v>
       </c>
@@ -6197,7 +6236,7 @@
       </c>
       <c r="AD55" s="14"/>
     </row>
-    <row r="56" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B56" s="28" t="s">
         <v>308</v>
       </c>
@@ -6229,7 +6268,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="57" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B57" s="21" t="s">
         <v>309</v>
       </c>
@@ -6261,7 +6300,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="58" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B58" s="28" t="s">
         <v>310</v>
       </c>
@@ -6293,7 +6332,7 @@
         <v>3205</v>
       </c>
     </row>
-    <row r="59" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B59" s="21" t="s">
         <v>311</v>
       </c>
@@ -6320,7 +6359,10 @@
       </c>
       <c r="AA59" s="39"/>
     </row>
-    <row r="60" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>719</v>
+      </c>
       <c r="B60" s="28" t="s">
         <v>312</v>
       </c>
@@ -6346,7 +6388,7 @@
       <c r="Y60" s="14"/>
       <c r="AA60" s="39"/>
     </row>
-    <row r="61" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B61" s="21" t="s">
         <v>313</v>
       </c>
@@ -6374,7 +6416,7 @@
       <c r="AA61" s="42"/>
       <c r="AC61" s="23"/>
     </row>
-    <row r="62" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B62" s="28" t="s">
         <v>314</v>
       </c>
@@ -6403,7 +6445,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="63" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B63" s="21" t="s">
         <v>315</v>
       </c>
@@ -6432,7 +6474,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="64" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B64" s="28" t="s">
         <v>316</v>
       </c>
@@ -6878,11 +6920,6 @@
     <sortCondition ref="C68"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="AU6:AX6"/>
-    <mergeCell ref="M1:AX1"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="T4:X4"/>
     <mergeCell ref="T16:X16"/>
     <mergeCell ref="T2:Y2"/>
     <mergeCell ref="B2:C2"/>
@@ -6890,6 +6927,11 @@
     <mergeCell ref="AD4:AI4"/>
     <mergeCell ref="AE33:AI33"/>
     <mergeCell ref="I8:K8"/>
+    <mergeCell ref="AU2:AX2"/>
+    <mergeCell ref="AU6:AX6"/>
+    <mergeCell ref="M1:AX1"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="T4:X4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AL17" r:id="rId1" display="https://www.orpha.net/consor/cgi-bin/Disease_Search.php?lng=FR&amp;data_id=11267&amp;Disease_Disease_Search_diseaseGroup=E53-8&amp;Disease_Disease_Search_diseaseType=ICD-10&amp;Maladie(s)/groupes%20de%20maladies=Deficit-en-biotinidase&amp;title=Déficit%20en%20biotinidase&amp;search=Disease_Search_Simple" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>